<commit_message>
QAPF map area 2a+2b
</commit_message>
<xml_diff>
--- a/_CIPW/CIPW/AREA2a/QAPF_counts.xlsx
+++ b/_CIPW/CIPW/AREA2a/QAPF_counts.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,7 +380,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>74650</v>
+        <v>79224</v>
       </c>
     </row>
     <row r="3">
@@ -390,7 +390,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5733</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="4">
@@ -401,17 +401,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1993</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>monzodiorite monzogabbro</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>140</v>
+        <v>542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>